<commit_message>
comit ok verção final
END.
</commit_message>
<xml_diff>
--- a/Requisitos e Casos de Uso 2.2.xlsx
+++ b/Requisitos e Casos de Uso 2.2.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -162,7 +157,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +169,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -199,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -222,6 +225,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,7 +530,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -534,7 +541,7 @@
   <dimension ref="A2:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E16" sqref="E15:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,25 +780,25 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="9">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="9">
         <v>10</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="9">
         <v>10</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="9" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>